<commit_message>
updated plots for analysis for items in Storyboard and report
</commit_message>
<xml_diff>
--- a/HeroesOfPymoli/HeroesOfPymoli_HW4_Storyboard.xlsx
+++ b/HeroesOfPymoli/HeroesOfPymoli_HW4_Storyboard.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18588" windowHeight="9335" firstSheet="5" activeTab="8"/>
+    <workbookView windowWidth="24348" windowHeight="12575" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="total_players" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="788">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1013" uniqueCount="788">
   <si>
     <t>total players</t>
   </si>
@@ -1854,16 +1854,16 @@
     <t>Oathbreaker, Last Hope of the Breaking Storm</t>
   </si>
   <si>
+    <t>Pursuit, Cudgel of Necromancy</t>
+  </si>
+  <si>
     <t>Fiery Glass Crusader</t>
   </si>
   <si>
+    <t>Nirvana</t>
+  </si>
+  <si>
     <t>Extraction, Quickblade Of Trembling Hands</t>
-  </si>
-  <si>
-    <t>Nirvana</t>
-  </si>
-  <si>
-    <t>Pursuit, Cudgel of Necromancy</t>
   </si>
   <si>
     <t>Singed Scalpel</t>
@@ -2395,10 +2395,10 @@
   <numFmts count="7">
     <numFmt numFmtId="176" formatCode="0_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
   </numFmts>
   <fonts count="21">
@@ -2433,41 +2433,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2503,8 +2470,64 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2512,6 +2535,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2526,37 +2556,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2571,19 +2571,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2595,13 +2613,91 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2619,13 +2715,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2637,19 +2739,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2661,97 +2751,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2789,15 +2789,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2828,17 +2819,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2858,6 +2854,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -2866,21 +2877,10 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2898,130 +2898,130 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7086,7 +7086,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="376092"/>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:lumMod val="75000"/>
+                </a:sysClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -7122,10 +7124,29 @@
               <a:effectLst/>
             </c:spPr>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="376092"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:dLbls>
             <c:dLbl>
               <c:idx val="0"/>
-              <c:layout/>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-0.00168067226890756"/>
+                  <c:y val="0.00221729490022173"/>
+                </c:manualLayout>
+              </c:layout>
               <c:tx>
                 <c:rich>
                   <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
@@ -7134,10 +7155,7 @@
                     <a:pPr defTabSz="914400">
                       <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                         <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
+                          <a:srgbClr val="FFFFFF"/>
                         </a:solidFill>
                         <a:uFill>
                           <a:solidFill>
@@ -7153,9 +7171,11 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr sz="1200" b="1">
+                      <a:rPr sz="1200" b="0">
                         <a:solidFill>
-                          <a:srgbClr val="FFFFFF"/>
+                          <a:schemeClr val="bg1">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
                         </a:solidFill>
                         <a:uFill>
                           <a:solidFill>
@@ -7166,11 +7186,13 @@
                           </a:solidFill>
                         </a:uFill>
                       </a:rPr>
-                      <a:t>Oathbreaker, Last Hope of the Breaking Storm</a:t>
+                      <a:t>Pursuit, Cudgel of Necromancy</a:t>
                     </a:r>
-                    <a:endParaRPr sz="1200" b="1">
+                    <a:endParaRPr sz="1200" b="0">
                       <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
+                        <a:schemeClr val="bg1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
                       </a:solidFill>
                       <a:uFill>
                         <a:solidFill>
@@ -7184,6 +7206,37 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                      <a:uFill>
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                      </a:uFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="inBase"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
@@ -7195,7 +7248,6 @@
                 <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                   <c15:layout/>
                   <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
                   <c15:showDataLabelsRange val="1"/>
                 </c:ext>
               </c:extLst>
@@ -7203,49 +7255,19 @@
             <c:dLbl>
               <c:idx val="1"/>
               <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr defTabSz="914400">
-                      <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:uFill>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:uFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr sz="1200" b="1">
-                        <a:solidFill>
-                          <a:srgbClr val="FFFFFF"/>
-                        </a:solidFill>
-                        <a:uFill>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:uFill>
-                      </a:rPr>
-                      <a:t>Fiery Glass Crusader</a:t>
-                    </a:r>
-                    <a:endParaRPr sz="1200" b="1">
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                       <a:solidFill>
                         <a:srgbClr val="FFFFFF"/>
                       </a:solidFill>
@@ -7257,10 +7279,13 @@
                           </a:schemeClr>
                         </a:solidFill>
                       </a:uFill>
-                    </a:endParaRPr>
-                  </a:p>
-                </c:rich>
-              </c:tx>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="inBase"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
@@ -7288,10 +7313,7 @@
                     <a:pPr defTabSz="914400">
                       <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                         <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
+                          <a:srgbClr val="FFFFFF"/>
                         </a:solidFill>
                         <a:uFill>
                           <a:solidFill>
@@ -7307,11 +7329,10 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr sz="1200">
+                      <a:rPr b="0">
                         <a:solidFill>
-                          <a:schemeClr val="tx1">
+                          <a:schemeClr val="bg1">
                             <a:lumMod val="50000"/>
-                            <a:lumOff val="50000"/>
                           </a:schemeClr>
                         </a:solidFill>
                         <a:uFill>
@@ -7325,11 +7346,10 @@
                       </a:rPr>
                       <a:t>Extraction, Quickblade Of Trembling Hands</a:t>
                     </a:r>
-                    <a:endParaRPr sz="1200">
+                    <a:endParaRPr b="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
+                        <a:schemeClr val="bg1">
                           <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
                         </a:schemeClr>
                       </a:solidFill>
                       <a:uFill>
@@ -7344,6 +7364,37 @@
                   </a:p>
                 </c:rich>
               </c:tx>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                      <a:solidFill>
+                        <a:srgbClr val="FFFFFF"/>
+                      </a:solidFill>
+                      <a:uFill>
+                        <a:solidFill>
+                          <a:schemeClr val="tx1">
+                            <a:lumMod val="75000"/>
+                            <a:lumOff val="25000"/>
+                          </a:schemeClr>
+                        </a:solidFill>
+                      </a:uFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="inBase"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
@@ -7363,49 +7414,19 @@
             <c:dLbl>
               <c:idx val="3"/>
               <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr defTabSz="914400">
-                      <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:uFill>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:uFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr sz="1200" b="1">
-                        <a:solidFill>
-                          <a:srgbClr val="FFFFFF"/>
-                        </a:solidFill>
-                        <a:uFill>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:uFill>
-                      </a:rPr>
-                      <a:t>Nirvana</a:t>
-                    </a:r>
-                    <a:endParaRPr sz="1200" b="1">
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                       <a:solidFill>
                         <a:srgbClr val="FFFFFF"/>
                       </a:solidFill>
@@ -7417,10 +7438,13 @@
                           </a:schemeClr>
                         </a:solidFill>
                       </a:uFill>
-                    </a:endParaRPr>
-                  </a:p>
-                </c:rich>
-              </c:tx>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="inBase"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
@@ -7440,57 +7464,21 @@
             <c:dLbl>
               <c:idx val="4"/>
               <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr defTabSz="914400">
-                      <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:uFill>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:uFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr sz="1200">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="50000"/>
-                            <a:lumOff val="50000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:uFill>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:uFill>
-                      </a:rPr>
-                      <a:t>Pursuit, Cudgel of Necromancy</a:t>
-                    </a:r>
-                    <a:endParaRPr sz="1200">
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                       <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
-                        </a:schemeClr>
+                        <a:srgbClr val="FFFFFF"/>
                       </a:solidFill>
                       <a:uFill>
                         <a:solidFill>
@@ -7500,10 +7488,13 @@
                           </a:schemeClr>
                         </a:solidFill>
                       </a:uFill>
-                    </a:endParaRPr>
-                  </a:p>
-                </c:rich>
-              </c:tx>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                </a:p>
+              </c:txPr>
               <c:dLblPos val="inBase"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
@@ -7520,7 +7511,6 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
-            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -7530,17 +7520,14 @@
             </c:spPr>
             <c:txPr>
               <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
+                <a:noAutofit/>
               </a:bodyPr>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                  <a:defRPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:srgbClr val="FFFFFF"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
@@ -7569,7 +7556,7 @@
               <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
                 <c15:layout/>
                 <c15:showDataLabelsRange val="1"/>
-                <c15:showLeaderLines val="1"/>
+                <c15:showLeaderLines val="0"/>
                 <c15:leaderLines>
                   <c:spPr>
                     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -7612,12 +7599,12 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>popular_df!$C$2:$C$6</c:f>
+              <c:f>popular_df!$I$2:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>9</c:v>
@@ -7629,7 +7616,7 @@
                   <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -7637,23 +7624,23 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>popular_df!$B$2:$B$6</c15:f>
+                <c15:f>popular_df!$H$2:$H$6</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>Oathbreaker, Last Hope of the Breaking Storm</c:v>
+                    <c:v>Pursuit, Cudgel of Necromancy</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Fiery Glass Crusader</c:v>
+                    <c:v>Nirvana</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>Extraction, Quickblade Of Trembling Hands</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Nirvana</c:v>
+                    <c:v>Fiery Glass Crusader</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Pursuit, Cudgel of Necromancy</c:v>
+                    <c:v>Oathbreaker, Last Hope of the Breaking Storm</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -7720,11 +7707,58 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr defTabSz="914400">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="1200">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:uFillTx/>
+                  </a:rPr>
+                  <a:t>Purchase </a:t>
+                </a:r>
+                <a:r>
+                  <a:t>count</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="high"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -7764,7 +7798,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="699077883"/>
-        <c:crosses val="autoZero"/>
+        <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -7849,7 +7883,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="376092"/>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:lumMod val="75000"/>
+                </a:sysClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -7863,7 +7899,9 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="376092"/>
+                <a:sysClr val="window" lastClr="FFFFFF">
+                  <a:lumMod val="75000"/>
+                </a:sysClr>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -7891,9 +7929,21 @@
             <c:bubble3D val="0"/>
             <c:spPr>
               <a:solidFill>
-                <a:sysClr val="window" lastClr="FFFFFF">
-                  <a:lumMod val="75000"/>
-                </a:sysClr>
+                <a:srgbClr val="376092"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
+          <c:dPt>
+            <c:idx val="4"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="376092"/>
               </a:solidFill>
               <a:ln>
                 <a:noFill/>
@@ -7913,10 +7963,7 @@
                     <a:pPr defTabSz="914400">
                       <a:defRPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                         <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
+                          <a:srgbClr val="FFFFFF"/>
                         </a:solidFill>
                         <a:uFill>
                           <a:solidFill>
@@ -7932,9 +7979,11 @@
                       </a:defRPr>
                     </a:pPr>
                     <a:r>
-                      <a:rPr sz="1200" b="1">
+                      <a:rPr sz="1200" b="0">
                         <a:solidFill>
-                          <a:srgbClr val="FFFFFF"/>
+                          <a:schemeClr val="bg1">
+                            <a:lumMod val="50000"/>
+                          </a:schemeClr>
                         </a:solidFill>
                         <a:uFill>
                           <a:solidFill>
@@ -7945,11 +7994,13 @@
                           </a:solidFill>
                         </a:uFill>
                       </a:rPr>
-                      <a:t>Oathbreaker, Last Hope of the Breaking Storm</a:t>
+                      <a:t>Singed Scalpel</a:t>
                     </a:r>
-                    <a:endParaRPr sz="1200" b="1">
+                    <a:endParaRPr sz="1200" b="0">
                       <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
+                        <a:schemeClr val="bg1">
+                          <a:lumMod val="50000"/>
+                        </a:schemeClr>
                       </a:solidFill>
                       <a:uFill>
                         <a:solidFill>
@@ -7963,40 +8014,6 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:uFill>
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                      </a:uFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
               <c:dLblPos val="inBase"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
@@ -8022,234 +8039,9 @@
                   <a:lstStyle/>
                   <a:p>
                     <a:pPr defTabSz="914400">
-                      <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:uFill>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:uFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr sz="1200" b="1">
+                      <a:defRPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                         <a:solidFill>
                           <a:srgbClr val="FFFFFF"/>
-                        </a:solidFill>
-                        <a:uFill>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:uFill>
-                      </a:rPr>
-                      <a:t>Nirvana</a:t>
-                    </a:r>
-                    <a:endParaRPr sz="1200" b="1">
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                      <a:uFill>
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                      </a:uFill>
-                    </a:endParaRPr>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:uFill>
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                      </a:uFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="inBase"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="2"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr defTabSz="914400">
-                      <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:uFill>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:uFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr sz="1200" b="1">
-                        <a:solidFill>
-                          <a:srgbClr val="FFFFFF"/>
-                        </a:solidFill>
-                        <a:uFill>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:uFill>
-                      </a:rPr>
-                      <a:t>Fiery Glass Crusader</a:t>
-                    </a:r>
-                    <a:endParaRPr sz="1200" b="1">
-                      <a:solidFill>
-                        <a:srgbClr val="FFFFFF"/>
-                      </a:solidFill>
-                      <a:uFill>
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                      </a:uFill>
-                    </a:endParaRPr>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:uFill>
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                      </a:uFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
-              <c:dLblPos val="inBase"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="0"/>
-              <c:showCatName val="0"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                  <c15:layout/>
-                  <c15:dlblFieldTable/>
-                  <c15:xForSave val="1"/>
-                  <c15:showDataLabelsRange val="1"/>
-                </c:ext>
-              </c:extLst>
-            </c:dLbl>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr defTabSz="914400">
-                      <a:defRPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
                         </a:solidFill>
                         <a:uFill>
                           <a:solidFill>
@@ -8302,40 +8094,44 @@
                   </a:p>
                 </c:rich>
               </c:tx>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:uFill>
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                      </a:uFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="2"/>
+              <c:layout/>
+              <c:dLblPos val="inBase"/>
+              <c:showLegendKey val="0"/>
+              <c:showVal val="0"/>
+              <c:showCatName val="0"/>
+              <c:showSerName val="0"/>
+              <c:showPercent val="0"/>
+              <c:showBubbleSize val="0"/>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                  <c15:layout/>
+                  <c15:dlblFieldTable/>
+                  <c15:xForSave val="1"/>
+                  <c15:showDataLabelsRange val="1"/>
+                </c:ext>
+              </c:extLst>
+            </c:dLbl>
+            <c:dLbl>
+              <c:idx val="3"/>
+              <c:layout/>
               <c:dLblPos val="inBase"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
@@ -8355,104 +8151,6 @@
             <c:dLbl>
               <c:idx val="4"/>
               <c:layout/>
-              <c:tx>
-                <c:rich>
-                  <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-                  <a:lstStyle/>
-                  <a:p>
-                    <a:pPr defTabSz="914400">
-                      <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:uFill>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:uFill>
-                        <a:latin typeface="+mn-lt"/>
-                        <a:ea typeface="+mn-ea"/>
-                        <a:cs typeface="+mn-cs"/>
-                      </a:defRPr>
-                    </a:pPr>
-                    <a:r>
-                      <a:rPr sz="1200">
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="50000"/>
-                            <a:lumOff val="50000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                        <a:uFill>
-                          <a:solidFill>
-                            <a:schemeClr val="tx1">
-                              <a:lumMod val="75000"/>
-                              <a:lumOff val="25000"/>
-                            </a:schemeClr>
-                          </a:solidFill>
-                        </a:uFill>
-                      </a:rPr>
-                      <a:t>Singed Scalpel</a:t>
-                    </a:r>
-                    <a:endParaRPr sz="1200">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="50000"/>
-                          <a:lumOff val="50000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:uFill>
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                      </a:uFill>
-                    </a:endParaRPr>
-                  </a:p>
-                </c:rich>
-              </c:tx>
-              <c:spPr>
-                <a:noFill/>
-                <a:ln>
-                  <a:noFill/>
-                </a:ln>
-                <a:effectLst/>
-              </c:spPr>
-              <c:txPr>
-                <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
-                <a:lstStyle/>
-                <a:p>
-                  <a:pPr>
-                    <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="75000"/>
-                          <a:lumOff val="25000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:uFill>
-                        <a:solidFill>
-                          <a:schemeClr val="tx1">
-                            <a:lumMod val="75000"/>
-                            <a:lumOff val="25000"/>
-                          </a:schemeClr>
-                        </a:solidFill>
-                      </a:uFill>
-                      <a:latin typeface="+mn-lt"/>
-                      <a:ea typeface="+mn-ea"/>
-                      <a:cs typeface="+mn-cs"/>
-                    </a:defRPr>
-                  </a:pPr>
-                </a:p>
-              </c:txPr>
               <c:dLblPos val="inBase"/>
               <c:showLegendKey val="0"/>
               <c:showVal val="0"/>
@@ -8469,6 +8167,7 @@
                 </c:ext>
               </c:extLst>
             </c:dLbl>
+            <c:numFmt formatCode="General" sourceLinked="1"/>
             <c:spPr>
               <a:noFill/>
               <a:ln>
@@ -8477,18 +8176,13 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:noAutofit/>
-              </a:bodyPr>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="none" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1"/>
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr lang="en-US" sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
+                  <a:defRPr lang="en-US" sz="1200" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                     <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
+                      <a:srgbClr val="FFFFFF"/>
                     </a:solidFill>
                     <a:uFill>
                       <a:solidFill>
@@ -8537,47 +8231,47 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>profitable_df!$B$2:$B$6</c:f>
+              <c:f>profitable_df!$H$2:$H$6</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>Oathbreaker, Last Hope of the Breaking Storm</c:v>
+                  <c:v>Singed Scalpel</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>Nirvana</c:v>
+                  <c:v>Final Critic</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>Fiery Glass Crusader</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>Final Critic</c:v>
+                  <c:v>Nirvana</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>Singed Scalpel</c:v>
+                  <c:v>Oathbreaker, Last Hope of the Breaking Storm</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>profitable_df!$E$2:$E$6</c:f>
+              <c:f>profitable_df!$I$2:$I$6</c:f>
               <c:numCache>
                 <c:formatCode>"$"#,##0.00_);[Red]\("$"#,##0.00\)</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>50.76</c:v>
+                  <c:v>34.8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44.1</c:v>
+                  <c:v>39.04</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>41.22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>39.04</c:v>
+                  <c:v>44.1</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>34.8</c:v>
+                  <c:v>50.76</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8585,23 +8279,23 @@
           <c:extLst>
             <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
               <c15:datalabelsRange>
-                <c15:f>profitable_df!$B$2:$B$6</c15:f>
+                <c15:f>profitable_df!$H$2:$H$6</c15:f>
                 <c15:dlblRangeCache>
                   <c:ptCount val="5"/>
                   <c:pt idx="0">
-                    <c:v>Oathbreaker, Last Hope of the Breaking Storm</c:v>
+                    <c:v>Singed Scalpel</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>Nirvana</c:v>
+                    <c:v>Final Critic</c:v>
                   </c:pt>
                   <c:pt idx="2">
                     <c:v>Fiery Glass Crusader</c:v>
                   </c:pt>
                   <c:pt idx="3">
-                    <c:v>Final Critic</c:v>
+                    <c:v>Nirvana</c:v>
                   </c:pt>
                   <c:pt idx="4">
-                    <c:v>Singed Scalpel</c:v>
+                    <c:v>Oathbreaker, Last Hope of the Breaking Storm</c:v>
                   </c:pt>
                 </c15:dlblRangeCache>
               </c15:datalabelsRange>
@@ -8668,11 +8362,64 @@
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="t"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="0" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr defTabSz="914400">
+                  <a:defRPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr sz="1200">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:uFillTx/>
+                  </a:rPr>
+                  <a:t>Total Purchase Value</a:t>
+                </a:r>
+                <a:endParaRPr sz="1200">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:uFillTx/>
+                </a:endParaRPr>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:title>
         <c:numFmt formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
+        <c:tickLblPos val="high"/>
         <c:spPr>
           <a:noFill/>
           <a:ln>
@@ -8712,7 +8459,7 @@
           </a:p>
         </c:txPr>
         <c:crossAx val="286120767"/>
-        <c:crosses val="autoZero"/>
+        <c:crosses val="max"/>
         <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
@@ -13219,16 +12966,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>490220</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>71120</xdr:rowOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>147320</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>109220</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>86360</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>33020</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>513080</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -13236,8 +12983,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="7203440" y="2997200"/>
-        <a:ext cx="4533900" cy="3436620"/>
+        <a:off x="7477760" y="1572260"/>
+        <a:ext cx="5486400" cy="3473450"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -13255,15 +13002,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>246380</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>170180</xdr:rowOff>
+      <xdr:colOff>360680</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>461010</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>360680</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>10160</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -13271,8 +13018,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="5763260" y="170180"/>
-        <a:ext cx="4535170" cy="3437890"/>
+        <a:off x="5877560" y="2570480"/>
+        <a:ext cx="5486400" cy="3474720"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -23443,19 +23190,21 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E184"/>
+  <dimension ref="A1:I184"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="P31" sqref="P31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N21" sqref="N21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="7.77777777777778" customWidth="1"/>
     <col min="2" max="2" width="44" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.5555555555556" customWidth="1"/>
     <col min="4" max="4" width="10.1111111111111" customWidth="1"/>
     <col min="5" max="5" width="20.4444444444444" customWidth="1"/>
+    <col min="8" max="8" width="44" customWidth="1"/>
+    <col min="9" max="9" width="3.66666666666667" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -23475,7 +23224,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:9">
       <c r="A2" s="3">
         <v>178</v>
       </c>
@@ -23491,13 +23240,19 @@
       <c r="E2">
         <v>50.76</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="H2" s="4" t="s">
+        <v>610</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="3">
         <v>145</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C3">
         <v>9</v>
@@ -23508,13 +23263,19 @@
       <c r="E3">
         <v>41.22</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="H3" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="I3">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="3">
         <v>108</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="C4">
         <v>9</v>
@@ -23525,8 +23286,14 @@
       <c r="E4">
         <v>31.77</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="H4" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="I4">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="3">
         <v>82</v>
       </c>
@@ -23542,13 +23309,19 @@
       <c r="E5">
         <v>44.1</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="H5" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="3">
         <v>19</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="C6">
         <v>8</v>
@@ -23558,6 +23331,12 @@
       </c>
       <c r="E6">
         <v>8.16</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -26596,19 +26375,20 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E184"/>
+  <dimension ref="A1:I184"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N29" sqref="N29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="4"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="7.77777777777778" customWidth="1"/>
     <col min="2" max="2" width="44" style="1" customWidth="1"/>
     <col min="3" max="3" width="5" customWidth="1"/>
     <col min="4" max="4" width="6.44444444444444" style="2" customWidth="1"/>
     <col min="5" max="5" width="8.22222222222222" style="2" customWidth="1"/>
+    <col min="8" max="8" width="44" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -26628,7 +26408,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:9">
       <c r="A2" s="3">
         <v>178</v>
       </c>
@@ -26644,8 +26424,14 @@
       <c r="E2" s="2">
         <v>50.76</v>
       </c>
-    </row>
-    <row r="3" spans="1:5">
+      <c r="H2" s="4" t="s">
+        <v>614</v>
+      </c>
+      <c r="I2" s="2">
+        <v>34.8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="3">
         <v>82</v>
       </c>
@@ -26661,13 +26447,19 @@
       <c r="E3" s="2">
         <v>44.1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5">
+      <c r="H3" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="I3" s="2">
+        <v>39.04</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9">
       <c r="A4" s="3">
         <v>145</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="C4">
         <v>9</v>
@@ -26678,8 +26470,14 @@
       <c r="E4" s="2">
         <v>41.22</v>
       </c>
-    </row>
-    <row r="5" spans="1:5">
+      <c r="H4" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="I4" s="2">
+        <v>41.22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="3">
         <v>92</v>
       </c>
@@ -26695,8 +26493,14 @@
       <c r="E5" s="2">
         <v>39.04</v>
       </c>
-    </row>
-    <row r="6" spans="1:5">
+      <c r="H5" s="4" t="s">
+        <v>612</v>
+      </c>
+      <c r="I5" s="2">
+        <v>44.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
       <c r="A6" s="3">
         <v>103</v>
       </c>
@@ -26711,6 +26515,12 @@
       </c>
       <c r="E6" s="2">
         <v>34.8</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>609</v>
+      </c>
+      <c r="I6" s="2">
+        <v>50.76</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -26735,7 +26545,7 @@
         <v>108</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>611</v>
+        <v>613</v>
       </c>
       <c r="C8">
         <v>9</v>
@@ -28775,7 +28585,7 @@
         <v>19</v>
       </c>
       <c r="B128" s="4" t="s">
-        <v>613</v>
+        <v>610</v>
       </c>
       <c r="C128">
         <v>8</v>

</xml_diff>